<commit_message>
feat: Add support for importing IAF codes from multiple Excel sheets
Extended import_iaf_codes command to read from both Sheet1 and Sheet11 in the Excel file. Added error handling for missing sheets with warning messages. Updated kodovi.xlsx file with additional data in Sheet11. Command now displays progress for each sheet and shows total count of imported groups and codes across all sheets.
</commit_message>
<xml_diff>
--- a/documents/kodovi.xlsx
+++ b/documents/kodovi.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVELOPER\ISOQAR\isoqar-app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD52148-4330-4220-AD73-15A968D45959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F257CD5-A1E7-4B8E-B513-F0C2C8D5F0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25755" yWindow="-15780" windowWidth="24000" windowHeight="14175" xr2:uid="{8EB7D492-D33E-4F9C-B4EF-0D9C64963CD2}"/>
+    <workbookView xWindow="25605" yWindow="-18960" windowWidth="24000" windowHeight="14175" xr2:uid="{8EB7D492-D33E-4F9C-B4EF-0D9C64963CD2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet11" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2827,10 +2827,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3166,849 +3166,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FDCEF4-CB77-430E-AF22-AE66FD1242FD}">
-  <dimension ref="A1:C90"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.90625" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>710</v>
-      </c>
-      <c r="B2" s="4">
-        <v>97.01</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="9"/>
-      <c r="B3" s="4">
-        <v>97.02</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9"/>
-      <c r="B4" s="4">
-        <v>97.03</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="9"/>
-      <c r="B5" s="4">
-        <v>97.04</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="9"/>
-      <c r="B6" s="4">
-        <v>97.05</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4">
-        <v>97.06</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="4">
-        <v>97.07</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="4">
-        <v>97.08</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="9"/>
-      <c r="B10" s="4">
-        <v>97.09</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="4">
-        <v>97.1</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="9"/>
-      <c r="B12" s="4">
-        <v>97.11</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="9"/>
-      <c r="B13" s="4">
-        <v>97.12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9"/>
-      <c r="B14" s="4">
-        <v>97.13</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9"/>
-      <c r="B15" s="4">
-        <v>97.14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="9"/>
-      <c r="B16" s="4">
-        <v>97.15</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="4">
-        <v>97.16</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="9"/>
-      <c r="B18" s="4">
-        <v>97.17</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9"/>
-      <c r="B19" s="4">
-        <v>97.18</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="4">
-        <v>97.19</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="9"/>
-      <c r="B21" s="4">
-        <v>97.2</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="4">
-        <v>97.21</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="9"/>
-      <c r="B23" s="4">
-        <v>97.22</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="4">
-        <v>97.23</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="4">
-        <v>97.24</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4">
-        <v>97.39</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="4">
-        <v>97.4</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="4">
-        <v>97.41</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="9"/>
-      <c r="B29" s="4">
-        <v>97.42</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="4">
-        <v>97.43</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="4">
-        <v>97.44</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="9"/>
-      <c r="B32" s="4">
-        <v>97.45</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="4">
-        <v>97.46</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="4">
-        <v>97.47</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="4">
-        <v>97.48</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="4">
-        <v>97.49</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="9"/>
-      <c r="B37" s="4">
-        <v>97.5</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="9"/>
-      <c r="B38" s="4">
-        <v>97.51</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="9"/>
-      <c r="B39" s="4">
-        <v>97.52</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="9"/>
-      <c r="B40" s="4">
-        <v>97.53</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="9"/>
-      <c r="B41" s="4">
-        <v>97.54</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="9"/>
-      <c r="B42" s="4">
-        <v>97.55</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="9"/>
-      <c r="B43" s="4">
-        <v>97.56</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="9"/>
-      <c r="B44" s="4">
-        <v>97.57</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="9"/>
-      <c r="B45" s="4">
-        <v>97.58</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="9"/>
-      <c r="B46" s="4">
-        <v>97.59</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="9"/>
-      <c r="B47" s="4">
-        <v>97.6</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="9"/>
-      <c r="B48" s="4">
-        <v>97.61</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="9"/>
-      <c r="B49" s="4">
-        <v>97.62</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="9"/>
-      <c r="B50" s="4">
-        <v>97.63</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="9"/>
-      <c r="B51" s="4">
-        <v>97.64</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="9"/>
-      <c r="B52" s="4">
-        <v>97.65</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="9"/>
-      <c r="B53" s="4">
-        <v>97.66</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="9"/>
-      <c r="B54" s="4">
-        <v>97.67</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="9"/>
-      <c r="B55" s="4">
-        <v>97.68</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="9"/>
-      <c r="B56" s="4">
-        <v>97.69</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="9"/>
-      <c r="B57" s="4">
-        <v>97.7</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="9"/>
-      <c r="B58" s="4">
-        <v>97.71</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="9"/>
-      <c r="B59" s="4">
-        <v>97.72</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="9"/>
-      <c r="B60" s="4">
-        <v>97.73</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="9"/>
-      <c r="B61" s="4">
-        <v>97.74</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="9"/>
-      <c r="B62" s="4">
-        <v>97.75</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="9"/>
-      <c r="B63" s="4">
-        <v>97.76</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="9"/>
-      <c r="B64" s="4">
-        <v>97.77</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="9"/>
-      <c r="B65" s="4">
-        <v>97.78</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="9"/>
-      <c r="B66" s="4">
-        <v>97.79</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="9"/>
-      <c r="B67" s="8">
-        <v>97.8</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="8" t="s">
-        <v>673</v>
-      </c>
-      <c r="B69" s="4">
-        <v>99.14</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="9"/>
-      <c r="B70" s="4">
-        <v>99.15</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="9"/>
-      <c r="B71" s="4">
-        <v>99.16</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="9"/>
-      <c r="B72" s="4">
-        <v>99.17</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="9"/>
-      <c r="B73" s="4" t="s">
-        <v>678</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="9"/>
-      <c r="B74" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="9"/>
-      <c r="B75" s="4" t="s">
-        <v>682</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="9"/>
-      <c r="B76" s="4" t="s">
-        <v>684</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="9"/>
-      <c r="B77" s="4" t="s">
-        <v>686</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="9"/>
-      <c r="B78" s="4" t="s">
-        <v>688</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="9"/>
-      <c r="B79" s="4">
-        <v>99.18</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="9"/>
-      <c r="B80" s="4" t="s">
-        <v>691</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="9"/>
-      <c r="B81" s="4" t="s">
-        <v>693</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="9"/>
-      <c r="B82" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="9"/>
-      <c r="B83" s="4" t="s">
-        <v>697</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="9"/>
-      <c r="B84" s="4">
-        <v>99.19</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="9"/>
-      <c r="B85" s="4">
-        <v>99.8</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="9"/>
-      <c r="B86" s="4" t="s">
-        <v>701</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="9"/>
-      <c r="B87" s="4" t="s">
-        <v>703</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="9"/>
-      <c r="B88" s="4">
-        <v>99.81</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="9"/>
-      <c r="B89" s="4" t="s">
-        <v>706</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="10"/>
-      <c r="B90" s="4" t="s">
-        <v>708</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>709</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A69:A90"/>
-    <mergeCell ref="A2:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF23E63-D207-4A71-AF51-9EF150AFDE59}">
   <dimension ref="A1:C671"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4906,7 +4068,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="15"/>
+      <c r="A140" s="16"/>
       <c r="B140" s="4" t="s">
         <v>95</v>
       </c>
@@ -5253,7 +4415,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A189" s="16"/>
+      <c r="A189" s="15"/>
       <c r="B189" s="4" t="s">
         <v>145</v>
       </c>
@@ -5262,7 +4424,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A190" s="16"/>
+      <c r="A190" s="15"/>
       <c r="B190" s="8" t="s">
         <v>147</v>
       </c>
@@ -5271,27 +4433,27 @@
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A191" s="16"/>
+      <c r="A191" s="15"/>
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192" s="16"/>
+      <c r="A192" s="15"/>
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193" s="16"/>
+      <c r="A193" s="15"/>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
     </row>
     <row r="194" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A194" s="16"/>
+      <c r="A194" s="15"/>
       <c r="B194" s="10"/>
       <c r="C194" s="10"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195" s="16"/>
+      <c r="A195" s="15"/>
       <c r="B195" s="8" t="s">
         <v>149</v>
       </c>
@@ -5300,27 +4462,27 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196" s="16"/>
+      <c r="A196" s="15"/>
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197" s="16"/>
+      <c r="A197" s="15"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A198" s="16"/>
+      <c r="A198" s="15"/>
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
     </row>
     <row r="199" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A199" s="16"/>
+      <c r="A199" s="15"/>
       <c r="B199" s="10"/>
       <c r="C199" s="10"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A200" s="16"/>
+      <c r="A200" s="15"/>
       <c r="B200" s="8" t="s">
         <v>151</v>
       </c>
@@ -5329,22 +4491,22 @@
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A201" s="16"/>
+      <c r="A201" s="15"/>
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A202" s="16"/>
+      <c r="A202" s="15"/>
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
     </row>
     <row r="203" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A203" s="16"/>
+      <c r="A203" s="15"/>
       <c r="B203" s="10"/>
       <c r="C203" s="10"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A204" s="16"/>
+      <c r="A204" s="15"/>
       <c r="B204" s="8" t="s">
         <v>153</v>
       </c>
@@ -5353,12 +4515,12 @@
       </c>
     </row>
     <row r="205" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A205" s="16"/>
+      <c r="A205" s="15"/>
       <c r="B205" s="10"/>
       <c r="C205" s="10"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A206" s="16"/>
+      <c r="A206" s="15"/>
       <c r="B206" s="8" t="s">
         <v>155</v>
       </c>
@@ -5367,12 +4529,12 @@
       </c>
     </row>
     <row r="207" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A207" s="16"/>
+      <c r="A207" s="15"/>
       <c r="B207" s="10"/>
       <c r="C207" s="10"/>
     </row>
     <row r="208" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A208" s="16"/>
+      <c r="A208" s="15"/>
       <c r="B208" s="4" t="s">
         <v>157</v>
       </c>
@@ -5381,7 +4543,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="16"/>
+      <c r="A209" s="15"/>
       <c r="B209" s="4" t="s">
         <v>159</v>
       </c>
@@ -5390,7 +4552,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A210" s="16"/>
+      <c r="A210" s="15"/>
       <c r="B210" s="8" t="s">
         <v>161</v>
       </c>
@@ -5399,12 +4561,12 @@
       </c>
     </row>
     <row r="211" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A211" s="16"/>
+      <c r="A211" s="15"/>
       <c r="B211" s="10"/>
       <c r="C211" s="10"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A212" s="16"/>
+      <c r="A212" s="15"/>
       <c r="B212" s="8" t="s">
         <v>163</v>
       </c>
@@ -5413,17 +4575,17 @@
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A213" s="16"/>
+      <c r="A213" s="15"/>
       <c r="B213" s="9"/>
       <c r="C213" s="9"/>
     </row>
     <row r="214" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A214" s="16"/>
+      <c r="A214" s="15"/>
       <c r="B214" s="10"/>
       <c r="C214" s="10"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A215" s="16"/>
+      <c r="A215" s="15"/>
       <c r="B215" s="8" t="s">
         <v>165</v>
       </c>
@@ -5432,27 +4594,27 @@
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A216" s="16"/>
+      <c r="A216" s="15"/>
       <c r="B216" s="9"/>
       <c r="C216" s="9"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A217" s="16"/>
+      <c r="A217" s="15"/>
       <c r="B217" s="9"/>
       <c r="C217" s="9"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A218" s="16"/>
+      <c r="A218" s="15"/>
       <c r="B218" s="9"/>
       <c r="C218" s="9"/>
     </row>
     <row r="219" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A219" s="16"/>
+      <c r="A219" s="15"/>
       <c r="B219" s="10"/>
       <c r="C219" s="10"/>
     </row>
     <row r="220" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A220" s="15"/>
+      <c r="A220" s="16"/>
       <c r="B220" s="4" t="s">
         <v>167</v>
       </c>
@@ -5737,7 +4899,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A260" s="12"/>
       <c r="B260" s="8" t="s">
         <v>210</v>
@@ -6287,12 +5449,12 @@
       </c>
     </row>
     <row r="333" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A333" s="16"/>
+      <c r="A333" s="15"/>
       <c r="B333" s="10"/>
       <c r="C333" s="10"/>
     </row>
     <row r="334" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A334" s="16"/>
+      <c r="A334" s="15"/>
       <c r="B334" s="4" t="s">
         <v>300</v>
       </c>
@@ -6301,7 +5463,7 @@
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A335" s="16"/>
+      <c r="A335" s="15"/>
       <c r="B335" s="8" t="s">
         <v>302</v>
       </c>
@@ -6310,12 +5472,12 @@
       </c>
     </row>
     <row r="336" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A336" s="16"/>
+      <c r="A336" s="15"/>
       <c r="B336" s="10"/>
       <c r="C336" s="10"/>
     </row>
     <row r="337" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A337" s="16"/>
+      <c r="A337" s="15"/>
       <c r="B337" s="4" t="s">
         <v>304</v>
       </c>
@@ -6324,7 +5486,7 @@
       </c>
     </row>
     <row r="338" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A338" s="16"/>
+      <c r="A338" s="15"/>
       <c r="B338" s="4" t="s">
         <v>306</v>
       </c>
@@ -6333,7 +5495,7 @@
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A339" s="16"/>
+      <c r="A339" s="15"/>
       <c r="B339" s="8" t="s">
         <v>308</v>
       </c>
@@ -6342,52 +5504,52 @@
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A340" s="16"/>
+      <c r="A340" s="15"/>
       <c r="B340" s="9"/>
       <c r="C340" s="9"/>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A341" s="16"/>
+      <c r="A341" s="15"/>
       <c r="B341" s="9"/>
       <c r="C341" s="9"/>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A342" s="16"/>
+      <c r="A342" s="15"/>
       <c r="B342" s="9"/>
       <c r="C342" s="9"/>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A343" s="16"/>
+      <c r="A343" s="15"/>
       <c r="B343" s="9"/>
       <c r="C343" s="9"/>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A344" s="16"/>
+      <c r="A344" s="15"/>
       <c r="B344" s="9"/>
       <c r="C344" s="9"/>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A345" s="16"/>
+      <c r="A345" s="15"/>
       <c r="B345" s="9"/>
       <c r="C345" s="9"/>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A346" s="16"/>
+      <c r="A346" s="15"/>
       <c r="B346" s="9"/>
       <c r="C346" s="9"/>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A347" s="16"/>
+      <c r="A347" s="15"/>
       <c r="B347" s="9"/>
       <c r="C347" s="9"/>
     </row>
     <row r="348" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A348" s="16"/>
+      <c r="A348" s="15"/>
       <c r="B348" s="10"/>
       <c r="C348" s="10"/>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A349" s="16"/>
+      <c r="A349" s="15"/>
       <c r="B349" s="8" t="s">
         <v>310</v>
       </c>
@@ -6396,22 +5558,22 @@
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A350" s="16"/>
+      <c r="A350" s="15"/>
       <c r="B350" s="9"/>
       <c r="C350" s="9"/>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A351" s="16"/>
+      <c r="A351" s="15"/>
       <c r="B351" s="9"/>
       <c r="C351" s="9"/>
     </row>
     <row r="352" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A352" s="16"/>
+      <c r="A352" s="15"/>
       <c r="B352" s="10"/>
       <c r="C352" s="10"/>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A353" s="16"/>
+      <c r="A353" s="15"/>
       <c r="B353" s="8" t="s">
         <v>312</v>
       </c>
@@ -6420,47 +5582,47 @@
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A354" s="16"/>
+      <c r="A354" s="15"/>
       <c r="B354" s="9"/>
       <c r="C354" s="9"/>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A355" s="16"/>
+      <c r="A355" s="15"/>
       <c r="B355" s="9"/>
       <c r="C355" s="9"/>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A356" s="16"/>
+      <c r="A356" s="15"/>
       <c r="B356" s="9"/>
       <c r="C356" s="9"/>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A357" s="16"/>
+      <c r="A357" s="15"/>
       <c r="B357" s="9"/>
       <c r="C357" s="9"/>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A358" s="16"/>
+      <c r="A358" s="15"/>
       <c r="B358" s="9"/>
       <c r="C358" s="9"/>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A359" s="16"/>
+      <c r="A359" s="15"/>
       <c r="B359" s="9"/>
       <c r="C359" s="9"/>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A360" s="16"/>
+      <c r="A360" s="15"/>
       <c r="B360" s="9"/>
       <c r="C360" s="9"/>
     </row>
     <row r="361" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A361" s="16"/>
+      <c r="A361" s="15"/>
       <c r="B361" s="10"/>
       <c r="C361" s="10"/>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A362" s="16"/>
+      <c r="A362" s="15"/>
       <c r="B362" s="8" t="s">
         <v>314</v>
       </c>
@@ -6469,47 +5631,47 @@
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A363" s="16"/>
+      <c r="A363" s="15"/>
       <c r="B363" s="9"/>
       <c r="C363" s="9"/>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A364" s="16"/>
+      <c r="A364" s="15"/>
       <c r="B364" s="9"/>
       <c r="C364" s="9"/>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A365" s="16"/>
+      <c r="A365" s="15"/>
       <c r="B365" s="9"/>
       <c r="C365" s="9"/>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A366" s="16"/>
+      <c r="A366" s="15"/>
       <c r="B366" s="9"/>
       <c r="C366" s="9"/>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A367" s="16"/>
+      <c r="A367" s="15"/>
       <c r="B367" s="9"/>
       <c r="C367" s="9"/>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A368" s="16"/>
+      <c r="A368" s="15"/>
       <c r="B368" s="9"/>
       <c r="C368" s="9"/>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A369" s="16"/>
+      <c r="A369" s="15"/>
       <c r="B369" s="9"/>
       <c r="C369" s="9"/>
     </row>
     <row r="370" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A370" s="16"/>
+      <c r="A370" s="15"/>
       <c r="B370" s="10"/>
       <c r="C370" s="10"/>
     </row>
     <row r="371" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A371" s="16"/>
+      <c r="A371" s="15"/>
       <c r="B371" s="4" t="s">
         <v>316</v>
       </c>
@@ -6518,7 +5680,7 @@
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A372" s="16"/>
+      <c r="A372" s="15"/>
       <c r="B372" s="8" t="s">
         <v>318</v>
       </c>
@@ -6527,42 +5689,42 @@
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A373" s="16"/>
+      <c r="A373" s="15"/>
       <c r="B373" s="9"/>
       <c r="C373" s="9"/>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A374" s="16"/>
+      <c r="A374" s="15"/>
       <c r="B374" s="9"/>
       <c r="C374" s="9"/>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A375" s="16"/>
+      <c r="A375" s="15"/>
       <c r="B375" s="9"/>
       <c r="C375" s="9"/>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A376" s="16"/>
+      <c r="A376" s="15"/>
       <c r="B376" s="9"/>
       <c r="C376" s="9"/>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A377" s="16"/>
+      <c r="A377" s="15"/>
       <c r="B377" s="9"/>
       <c r="C377" s="9"/>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A378" s="16"/>
+      <c r="A378" s="15"/>
       <c r="B378" s="9"/>
       <c r="C378" s="9"/>
     </row>
     <row r="379" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A379" s="16"/>
+      <c r="A379" s="15"/>
       <c r="B379" s="10"/>
       <c r="C379" s="10"/>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A380" s="16"/>
+      <c r="A380" s="15"/>
       <c r="B380" s="8" t="s">
         <v>320</v>
       </c>
@@ -6571,37 +5733,37 @@
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A381" s="16"/>
+      <c r="A381" s="15"/>
       <c r="B381" s="9"/>
       <c r="C381" s="9"/>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A382" s="16"/>
+      <c r="A382" s="15"/>
       <c r="B382" s="9"/>
       <c r="C382" s="9"/>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A383" s="16"/>
+      <c r="A383" s="15"/>
       <c r="B383" s="9"/>
       <c r="C383" s="9"/>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A384" s="16"/>
+      <c r="A384" s="15"/>
       <c r="B384" s="9"/>
       <c r="C384" s="9"/>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A385" s="16"/>
+      <c r="A385" s="15"/>
       <c r="B385" s="9"/>
       <c r="C385" s="9"/>
     </row>
     <row r="386" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A386" s="16"/>
+      <c r="A386" s="15"/>
       <c r="B386" s="10"/>
       <c r="C386" s="10"/>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A387" s="16"/>
+      <c r="A387" s="15"/>
       <c r="B387" s="8" t="s">
         <v>322</v>
       </c>
@@ -6610,12 +5772,12 @@
       </c>
     </row>
     <row r="388" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A388" s="16"/>
+      <c r="A388" s="15"/>
       <c r="B388" s="10"/>
       <c r="C388" s="10"/>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A389" s="16"/>
+      <c r="A389" s="15"/>
       <c r="B389" s="8" t="s">
         <v>324</v>
       </c>
@@ -6624,42 +5786,42 @@
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A390" s="16"/>
+      <c r="A390" s="15"/>
       <c r="B390" s="9"/>
       <c r="C390" s="9"/>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A391" s="16"/>
+      <c r="A391" s="15"/>
       <c r="B391" s="9"/>
       <c r="C391" s="9"/>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A392" s="16"/>
+      <c r="A392" s="15"/>
       <c r="B392" s="9"/>
       <c r="C392" s="9"/>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A393" s="16"/>
+      <c r="A393" s="15"/>
       <c r="B393" s="9"/>
       <c r="C393" s="9"/>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A394" s="16"/>
+      <c r="A394" s="15"/>
       <c r="B394" s="9"/>
       <c r="C394" s="9"/>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A395" s="16"/>
+      <c r="A395" s="15"/>
       <c r="B395" s="9"/>
       <c r="C395" s="9"/>
     </row>
     <row r="396" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A396" s="16"/>
+      <c r="A396" s="15"/>
       <c r="B396" s="10"/>
       <c r="C396" s="10"/>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A397" s="16"/>
+      <c r="A397" s="15"/>
       <c r="B397" s="8" t="s">
         <v>326</v>
       </c>
@@ -6668,32 +5830,32 @@
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A398" s="16"/>
+      <c r="A398" s="15"/>
       <c r="B398" s="9"/>
       <c r="C398" s="9"/>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A399" s="16"/>
+      <c r="A399" s="15"/>
       <c r="B399" s="9"/>
       <c r="C399" s="9"/>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A400" s="16"/>
+      <c r="A400" s="15"/>
       <c r="B400" s="9"/>
       <c r="C400" s="9"/>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A401" s="16"/>
+      <c r="A401" s="15"/>
       <c r="B401" s="9"/>
       <c r="C401" s="9"/>
     </row>
     <row r="402" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A402" s="16"/>
+      <c r="A402" s="15"/>
       <c r="B402" s="10"/>
       <c r="C402" s="10"/>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A403" s="16"/>
+      <c r="A403" s="15"/>
       <c r="B403" s="8" t="s">
         <v>328</v>
       </c>
@@ -6702,52 +5864,52 @@
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A404" s="16"/>
+      <c r="A404" s="15"/>
       <c r="B404" s="9"/>
       <c r="C404" s="9"/>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A405" s="16"/>
+      <c r="A405" s="15"/>
       <c r="B405" s="9"/>
       <c r="C405" s="9"/>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A406" s="16"/>
+      <c r="A406" s="15"/>
       <c r="B406" s="9"/>
       <c r="C406" s="9"/>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A407" s="16"/>
+      <c r="A407" s="15"/>
       <c r="B407" s="9"/>
       <c r="C407" s="9"/>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A408" s="16"/>
+      <c r="A408" s="15"/>
       <c r="B408" s="9"/>
       <c r="C408" s="9"/>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A409" s="16"/>
+      <c r="A409" s="15"/>
       <c r="B409" s="9"/>
       <c r="C409" s="9"/>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A410" s="16"/>
+      <c r="A410" s="15"/>
       <c r="B410" s="9"/>
       <c r="C410" s="9"/>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A411" s="16"/>
+      <c r="A411" s="15"/>
       <c r="B411" s="9"/>
       <c r="C411" s="9"/>
     </row>
     <row r="412" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A412" s="16"/>
+      <c r="A412" s="15"/>
       <c r="B412" s="10"/>
       <c r="C412" s="10"/>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A413" s="16"/>
+      <c r="A413" s="15"/>
       <c r="B413" s="8" t="s">
         <v>330</v>
       </c>
@@ -6756,27 +5918,27 @@
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A414" s="16"/>
+      <c r="A414" s="15"/>
       <c r="B414" s="9"/>
       <c r="C414" s="9"/>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A415" s="16"/>
+      <c r="A415" s="15"/>
       <c r="B415" s="9"/>
       <c r="C415" s="9"/>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A416" s="16"/>
+      <c r="A416" s="15"/>
       <c r="B416" s="9"/>
       <c r="C416" s="9"/>
     </row>
     <row r="417" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A417" s="16"/>
+      <c r="A417" s="15"/>
       <c r="B417" s="10"/>
       <c r="C417" s="10"/>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A418" s="16"/>
+      <c r="A418" s="15"/>
       <c r="B418" s="8" t="s">
         <v>332</v>
       </c>
@@ -6785,12 +5947,12 @@
       </c>
     </row>
     <row r="419" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A419" s="16"/>
+      <c r="A419" s="15"/>
       <c r="B419" s="10"/>
       <c r="C419" s="10"/>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A420" s="16"/>
+      <c r="A420" s="15"/>
       <c r="B420" s="8" t="s">
         <v>334</v>
       </c>
@@ -6799,32 +5961,32 @@
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A421" s="16"/>
+      <c r="A421" s="15"/>
       <c r="B421" s="9"/>
       <c r="C421" s="9"/>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A422" s="16"/>
+      <c r="A422" s="15"/>
       <c r="B422" s="9"/>
       <c r="C422" s="9"/>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A423" s="16"/>
+      <c r="A423" s="15"/>
       <c r="B423" s="9"/>
       <c r="C423" s="9"/>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A424" s="16"/>
+      <c r="A424" s="15"/>
       <c r="B424" s="9"/>
       <c r="C424" s="9"/>
     </row>
     <row r="425" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A425" s="16"/>
+      <c r="A425" s="15"/>
       <c r="B425" s="10"/>
       <c r="C425" s="10"/>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A426" s="16"/>
+      <c r="A426" s="15"/>
       <c r="B426" s="8" t="s">
         <v>336</v>
       </c>
@@ -6833,12 +5995,12 @@
       </c>
     </row>
     <row r="427" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A427" s="16"/>
+      <c r="A427" s="15"/>
       <c r="B427" s="10"/>
       <c r="C427" s="10"/>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A428" s="16"/>
+      <c r="A428" s="15"/>
       <c r="B428" s="8" t="s">
         <v>338</v>
       </c>
@@ -6847,17 +6009,17 @@
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A429" s="16"/>
+      <c r="A429" s="15"/>
       <c r="B429" s="9"/>
       <c r="C429" s="9"/>
     </row>
     <row r="430" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A430" s="16"/>
+      <c r="A430" s="15"/>
       <c r="B430" s="10"/>
       <c r="C430" s="10"/>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A431" s="16"/>
+      <c r="A431" s="15"/>
       <c r="B431" s="8" t="s">
         <v>340</v>
       </c>
@@ -6866,12 +6028,12 @@
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A432" s="16"/>
+      <c r="A432" s="15"/>
       <c r="B432" s="9"/>
       <c r="C432" s="9"/>
     </row>
     <row r="433" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A433" s="15"/>
+      <c r="A433" s="16"/>
       <c r="B433" s="10"/>
       <c r="C433" s="10"/>
     </row>
@@ -7158,12 +6320,12 @@
       </c>
     </row>
     <row r="470" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A470" s="16"/>
+      <c r="A470" s="15"/>
       <c r="B470" s="10"/>
       <c r="C470" s="10"/>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A471" s="16"/>
+      <c r="A471" s="15"/>
       <c r="B471" s="8" t="s">
         <v>392</v>
       </c>
@@ -7172,12 +6334,12 @@
       </c>
     </row>
     <row r="472" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A472" s="16"/>
+      <c r="A472" s="15"/>
       <c r="B472" s="10"/>
       <c r="C472" s="10"/>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A473" s="16"/>
+      <c r="A473" s="15"/>
       <c r="B473" s="8" t="s">
         <v>394</v>
       </c>
@@ -7186,22 +6348,22 @@
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A474" s="16"/>
+      <c r="A474" s="15"/>
       <c r="B474" s="9"/>
       <c r="C474" s="9"/>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A475" s="16"/>
+      <c r="A475" s="15"/>
       <c r="B475" s="9"/>
       <c r="C475" s="9"/>
     </row>
     <row r="476" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A476" s="16"/>
+      <c r="A476" s="15"/>
       <c r="B476" s="10"/>
       <c r="C476" s="10"/>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A477" s="16"/>
+      <c r="A477" s="15"/>
       <c r="B477" s="8" t="s">
         <v>396</v>
       </c>
@@ -7210,22 +6372,22 @@
       </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A478" s="16"/>
+      <c r="A478" s="15"/>
       <c r="B478" s="9"/>
       <c r="C478" s="9"/>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A479" s="16"/>
+      <c r="A479" s="15"/>
       <c r="B479" s="9"/>
       <c r="C479" s="9"/>
     </row>
     <row r="480" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A480" s="16"/>
+      <c r="A480" s="15"/>
       <c r="B480" s="10"/>
       <c r="C480" s="10"/>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A481" s="16"/>
+      <c r="A481" s="15"/>
       <c r="B481" s="8" t="s">
         <v>398</v>
       </c>
@@ -7234,17 +6396,17 @@
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A482" s="16"/>
+      <c r="A482" s="15"/>
       <c r="B482" s="9"/>
       <c r="C482" s="9"/>
     </row>
     <row r="483" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A483" s="16"/>
+      <c r="A483" s="15"/>
       <c r="B483" s="10"/>
       <c r="C483" s="10"/>
     </row>
     <row r="484" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A484" s="16"/>
+      <c r="A484" s="15"/>
       <c r="B484" s="4" t="s">
         <v>400</v>
       </c>
@@ -7253,7 +6415,7 @@
       </c>
     </row>
     <row r="485" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A485" s="16"/>
+      <c r="A485" s="15"/>
       <c r="B485" s="4" t="s">
         <v>402</v>
       </c>
@@ -7262,7 +6424,7 @@
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A486" s="16"/>
+      <c r="A486" s="15"/>
       <c r="B486" s="8" t="s">
         <v>404</v>
       </c>
@@ -7271,12 +6433,12 @@
       </c>
     </row>
     <row r="487" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A487" s="16"/>
+      <c r="A487" s="15"/>
       <c r="B487" s="10"/>
       <c r="C487" s="10"/>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A488" s="16"/>
+      <c r="A488" s="15"/>
       <c r="B488" s="8" t="s">
         <v>406</v>
       </c>
@@ -7285,12 +6447,12 @@
       </c>
     </row>
     <row r="489" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A489" s="16"/>
+      <c r="A489" s="15"/>
       <c r="B489" s="10"/>
       <c r="C489" s="10"/>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A490" s="16"/>
+      <c r="A490" s="15"/>
       <c r="B490" s="8" t="s">
         <v>408</v>
       </c>
@@ -7299,17 +6461,17 @@
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A491" s="16"/>
+      <c r="A491" s="15"/>
       <c r="B491" s="9"/>
       <c r="C491" s="9"/>
     </row>
     <row r="492" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A492" s="16"/>
+      <c r="A492" s="15"/>
       <c r="B492" s="10"/>
       <c r="C492" s="10"/>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A493" s="16"/>
+      <c r="A493" s="15"/>
       <c r="B493" s="8" t="s">
         <v>410</v>
       </c>
@@ -7318,32 +6480,32 @@
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A494" s="16"/>
+      <c r="A494" s="15"/>
       <c r="B494" s="9"/>
       <c r="C494" s="9"/>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A495" s="16"/>
+      <c r="A495" s="15"/>
       <c r="B495" s="9"/>
       <c r="C495" s="9"/>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A496" s="16"/>
+      <c r="A496" s="15"/>
       <c r="B496" s="9"/>
       <c r="C496" s="9"/>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A497" s="16"/>
+      <c r="A497" s="15"/>
       <c r="B497" s="9"/>
       <c r="C497" s="9"/>
     </row>
     <row r="498" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A498" s="16"/>
+      <c r="A498" s="15"/>
       <c r="B498" s="10"/>
       <c r="C498" s="10"/>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A499" s="16"/>
+      <c r="A499" s="15"/>
       <c r="B499" s="8" t="s">
         <v>412</v>
       </c>
@@ -7352,17 +6514,17 @@
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A500" s="16"/>
+      <c r="A500" s="15"/>
       <c r="B500" s="9"/>
       <c r="C500" s="9"/>
     </row>
     <row r="501" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A501" s="16"/>
+      <c r="A501" s="15"/>
       <c r="B501" s="10"/>
       <c r="C501" s="10"/>
     </row>
     <row r="502" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A502" s="16"/>
+      <c r="A502" s="15"/>
       <c r="B502" s="4" t="s">
         <v>414</v>
       </c>
@@ -7371,7 +6533,7 @@
       </c>
     </row>
     <row r="503" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A503" s="15"/>
+      <c r="A503" s="16"/>
       <c r="B503" s="4" t="s">
         <v>416</v>
       </c>
@@ -8536,7 +7698,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="655" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="655" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A655" s="9"/>
       <c r="B655" s="4">
         <v>96.04</v>
@@ -8691,6 +7853,294 @@
     </row>
   </sheetData>
   <mergeCells count="312">
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="A41:A57"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="C49:C55"/>
+    <mergeCell ref="A2:A40"/>
+    <mergeCell ref="B2:B19"/>
+    <mergeCell ref="C2:C19"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="C20:C28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A113:A119"/>
+    <mergeCell ref="B114:B119"/>
+    <mergeCell ref="C114:C119"/>
+    <mergeCell ref="B80:B86"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="A92:A109"/>
+    <mergeCell ref="B95:B99"/>
+    <mergeCell ref="C95:C99"/>
+    <mergeCell ref="B100:B106"/>
+    <mergeCell ref="C100:C106"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="A58:A91"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="B73:B79"/>
+    <mergeCell ref="C73:C79"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="A142:A157"/>
+    <mergeCell ref="B142:B148"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="C153:C156"/>
+    <mergeCell ref="A120:A127"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="B122:B127"/>
+    <mergeCell ref="C122:C127"/>
+    <mergeCell ref="A128:A133"/>
+    <mergeCell ref="B128:B132"/>
+    <mergeCell ref="C128:C132"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A166:A180"/>
+    <mergeCell ref="B166:B170"/>
+    <mergeCell ref="C166:C170"/>
+    <mergeCell ref="B172:B173"/>
+    <mergeCell ref="C172:C173"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="C174:C178"/>
+    <mergeCell ref="A158:A159"/>
+    <mergeCell ref="A160:A165"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="B162:B165"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="B200:B203"/>
+    <mergeCell ref="C200:C203"/>
+    <mergeCell ref="B204:B205"/>
+    <mergeCell ref="C204:C205"/>
+    <mergeCell ref="B206:B207"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="A181:A187"/>
+    <mergeCell ref="B182:B187"/>
+    <mergeCell ref="C182:C187"/>
+    <mergeCell ref="B190:B194"/>
+    <mergeCell ref="C190:C194"/>
+    <mergeCell ref="B195:B199"/>
+    <mergeCell ref="C195:C199"/>
+    <mergeCell ref="A188:A220"/>
+    <mergeCell ref="A221:A245"/>
+    <mergeCell ref="B221:B225"/>
+    <mergeCell ref="C221:C225"/>
+    <mergeCell ref="B226:B232"/>
+    <mergeCell ref="C226:C232"/>
+    <mergeCell ref="B235:B241"/>
+    <mergeCell ref="C235:C241"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="B212:B214"/>
+    <mergeCell ref="C212:C214"/>
+    <mergeCell ref="B215:B219"/>
+    <mergeCell ref="C215:C219"/>
+    <mergeCell ref="C268:C269"/>
+    <mergeCell ref="A270:A272"/>
+    <mergeCell ref="B270:B271"/>
+    <mergeCell ref="C270:C271"/>
+    <mergeCell ref="A273:A274"/>
+    <mergeCell ref="A275:A284"/>
+    <mergeCell ref="B276:B277"/>
+    <mergeCell ref="B278:B279"/>
+    <mergeCell ref="C278:C279"/>
+    <mergeCell ref="B281:B283"/>
+    <mergeCell ref="A246:A269"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="B249:B250"/>
+    <mergeCell ref="C249:C250"/>
+    <mergeCell ref="B251:B253"/>
+    <mergeCell ref="C251:C253"/>
+    <mergeCell ref="B260:B261"/>
+    <mergeCell ref="B262:B263"/>
+    <mergeCell ref="C262:C263"/>
+    <mergeCell ref="B268:B269"/>
+    <mergeCell ref="A299:A300"/>
+    <mergeCell ref="B299:B300"/>
+    <mergeCell ref="C299:C300"/>
+    <mergeCell ref="A301:A304"/>
+    <mergeCell ref="B301:B304"/>
+    <mergeCell ref="C301:C304"/>
+    <mergeCell ref="C281:C283"/>
+    <mergeCell ref="A285:A298"/>
+    <mergeCell ref="B285:B288"/>
+    <mergeCell ref="C285:C288"/>
+    <mergeCell ref="B289:B291"/>
+    <mergeCell ref="C289:C291"/>
+    <mergeCell ref="B295:B296"/>
+    <mergeCell ref="C295:C296"/>
+    <mergeCell ref="A305:A307"/>
+    <mergeCell ref="B305:B307"/>
+    <mergeCell ref="C305:C307"/>
+    <mergeCell ref="A308:A309"/>
+    <mergeCell ref="A310:A331"/>
+    <mergeCell ref="B310:B312"/>
+    <mergeCell ref="C310:C312"/>
+    <mergeCell ref="B314:B316"/>
+    <mergeCell ref="C314:C316"/>
+    <mergeCell ref="B317:B321"/>
+    <mergeCell ref="B330:B331"/>
+    <mergeCell ref="C330:C331"/>
+    <mergeCell ref="B332:B333"/>
+    <mergeCell ref="C332:C333"/>
+    <mergeCell ref="B335:B336"/>
+    <mergeCell ref="C335:C336"/>
+    <mergeCell ref="C317:C321"/>
+    <mergeCell ref="B323:B325"/>
+    <mergeCell ref="C323:C325"/>
+    <mergeCell ref="B326:B327"/>
+    <mergeCell ref="C326:C327"/>
+    <mergeCell ref="B328:B329"/>
+    <mergeCell ref="C328:C329"/>
+    <mergeCell ref="B397:B402"/>
+    <mergeCell ref="C397:C402"/>
+    <mergeCell ref="B362:B370"/>
+    <mergeCell ref="C362:C370"/>
+    <mergeCell ref="B372:B379"/>
+    <mergeCell ref="C372:C379"/>
+    <mergeCell ref="B380:B386"/>
+    <mergeCell ref="C380:C386"/>
+    <mergeCell ref="B339:B348"/>
+    <mergeCell ref="C339:C348"/>
+    <mergeCell ref="B349:B352"/>
+    <mergeCell ref="C349:C352"/>
+    <mergeCell ref="B353:B361"/>
+    <mergeCell ref="C353:C361"/>
+    <mergeCell ref="B431:B433"/>
+    <mergeCell ref="C431:C433"/>
+    <mergeCell ref="A434:A441"/>
+    <mergeCell ref="B434:B436"/>
+    <mergeCell ref="C434:C436"/>
+    <mergeCell ref="B440:B441"/>
+    <mergeCell ref="C440:C441"/>
+    <mergeCell ref="B420:B425"/>
+    <mergeCell ref="C420:C425"/>
+    <mergeCell ref="B426:B427"/>
+    <mergeCell ref="C426:C427"/>
+    <mergeCell ref="B428:B430"/>
+    <mergeCell ref="C428:C430"/>
+    <mergeCell ref="A332:A433"/>
+    <mergeCell ref="B403:B412"/>
+    <mergeCell ref="C403:C412"/>
+    <mergeCell ref="B413:B417"/>
+    <mergeCell ref="C413:C417"/>
+    <mergeCell ref="B418:B419"/>
+    <mergeCell ref="C418:C419"/>
+    <mergeCell ref="B387:B388"/>
+    <mergeCell ref="C387:C388"/>
+    <mergeCell ref="B389:B396"/>
+    <mergeCell ref="C389:C396"/>
+    <mergeCell ref="C465:C467"/>
+    <mergeCell ref="B469:B470"/>
+    <mergeCell ref="C469:C470"/>
+    <mergeCell ref="B471:B472"/>
+    <mergeCell ref="C471:C472"/>
+    <mergeCell ref="B473:B476"/>
+    <mergeCell ref="C473:C476"/>
+    <mergeCell ref="A442:A468"/>
+    <mergeCell ref="B443:B444"/>
+    <mergeCell ref="C443:C444"/>
+    <mergeCell ref="B446:B447"/>
+    <mergeCell ref="C446:C447"/>
+    <mergeCell ref="B450:B451"/>
+    <mergeCell ref="C450:C451"/>
+    <mergeCell ref="B454:B458"/>
+    <mergeCell ref="C454:C458"/>
+    <mergeCell ref="B465:B467"/>
+    <mergeCell ref="A469:A503"/>
+    <mergeCell ref="B488:B489"/>
+    <mergeCell ref="C488:C489"/>
+    <mergeCell ref="B490:B492"/>
+    <mergeCell ref="C490:C492"/>
+    <mergeCell ref="B493:B498"/>
+    <mergeCell ref="C493:C498"/>
+    <mergeCell ref="B477:B480"/>
+    <mergeCell ref="C477:C480"/>
+    <mergeCell ref="B481:B483"/>
+    <mergeCell ref="C481:C483"/>
+    <mergeCell ref="B486:B487"/>
+    <mergeCell ref="C486:C487"/>
+    <mergeCell ref="B499:B501"/>
+    <mergeCell ref="C499:C501"/>
+    <mergeCell ref="A504:A511"/>
+    <mergeCell ref="B504:B505"/>
+    <mergeCell ref="C504:C505"/>
+    <mergeCell ref="B506:B509"/>
+    <mergeCell ref="C506:C509"/>
+    <mergeCell ref="B510:B511"/>
+    <mergeCell ref="C510:C511"/>
+    <mergeCell ref="B525:B526"/>
+    <mergeCell ref="C525:C526"/>
+    <mergeCell ref="B528:B530"/>
+    <mergeCell ref="C528:C530"/>
+    <mergeCell ref="B541:B543"/>
+    <mergeCell ref="C541:C543"/>
+    <mergeCell ref="A512:A519"/>
+    <mergeCell ref="B512:B513"/>
+    <mergeCell ref="C512:C513"/>
+    <mergeCell ref="B515:B516"/>
+    <mergeCell ref="C515:C516"/>
+    <mergeCell ref="A520:A548"/>
+    <mergeCell ref="B520:B521"/>
+    <mergeCell ref="C520:C521"/>
+    <mergeCell ref="B523:B524"/>
+    <mergeCell ref="C523:C524"/>
+    <mergeCell ref="B546:B548"/>
+    <mergeCell ref="C546:C548"/>
+    <mergeCell ref="A559:A569"/>
+    <mergeCell ref="B560:B561"/>
+    <mergeCell ref="C560:C561"/>
+    <mergeCell ref="B562:B563"/>
+    <mergeCell ref="C562:C563"/>
+    <mergeCell ref="B564:B567"/>
+    <mergeCell ref="C564:C567"/>
+    <mergeCell ref="A549:A558"/>
+    <mergeCell ref="B549:B552"/>
+    <mergeCell ref="C549:C552"/>
+    <mergeCell ref="B553:B557"/>
+    <mergeCell ref="C553:C557"/>
+    <mergeCell ref="C597:C600"/>
+    <mergeCell ref="B601:B602"/>
+    <mergeCell ref="C601:C602"/>
+    <mergeCell ref="B603:B606"/>
+    <mergeCell ref="C603:C606"/>
+    <mergeCell ref="B607:B610"/>
+    <mergeCell ref="C607:C610"/>
+    <mergeCell ref="B597:B600"/>
+    <mergeCell ref="A570:A583"/>
+    <mergeCell ref="B572:B574"/>
+    <mergeCell ref="C572:C574"/>
+    <mergeCell ref="B577:B578"/>
+    <mergeCell ref="B582:B583"/>
+    <mergeCell ref="C582:C583"/>
     <mergeCell ref="A637:A647"/>
     <mergeCell ref="A648:A651"/>
     <mergeCell ref="A652:A671"/>
@@ -8715,296 +8165,846 @@
     <mergeCell ref="C613:C617"/>
     <mergeCell ref="B619:B620"/>
     <mergeCell ref="C619:C620"/>
-    <mergeCell ref="C597:C600"/>
-    <mergeCell ref="B601:B602"/>
-    <mergeCell ref="C601:C602"/>
-    <mergeCell ref="B603:B606"/>
-    <mergeCell ref="C603:C606"/>
-    <mergeCell ref="B607:B610"/>
-    <mergeCell ref="C607:C610"/>
-    <mergeCell ref="B597:B600"/>
-    <mergeCell ref="A570:A583"/>
-    <mergeCell ref="B572:B574"/>
-    <mergeCell ref="C572:C574"/>
-    <mergeCell ref="B577:B578"/>
-    <mergeCell ref="B582:B583"/>
-    <mergeCell ref="C582:C583"/>
-    <mergeCell ref="A559:A569"/>
-    <mergeCell ref="B560:B561"/>
-    <mergeCell ref="C560:C561"/>
-    <mergeCell ref="B562:B563"/>
-    <mergeCell ref="C562:C563"/>
-    <mergeCell ref="B564:B567"/>
-    <mergeCell ref="C564:C567"/>
-    <mergeCell ref="A549:A558"/>
-    <mergeCell ref="B549:B552"/>
-    <mergeCell ref="C549:C552"/>
-    <mergeCell ref="B553:B557"/>
-    <mergeCell ref="C553:C557"/>
-    <mergeCell ref="B525:B526"/>
-    <mergeCell ref="C525:C526"/>
-    <mergeCell ref="B528:B530"/>
-    <mergeCell ref="C528:C530"/>
-    <mergeCell ref="B541:B543"/>
-    <mergeCell ref="C541:C543"/>
-    <mergeCell ref="A512:A519"/>
-    <mergeCell ref="B512:B513"/>
-    <mergeCell ref="C512:C513"/>
-    <mergeCell ref="B515:B516"/>
-    <mergeCell ref="C515:C516"/>
-    <mergeCell ref="A520:A548"/>
-    <mergeCell ref="B520:B521"/>
-    <mergeCell ref="C520:C521"/>
-    <mergeCell ref="B523:B524"/>
-    <mergeCell ref="C523:C524"/>
-    <mergeCell ref="B546:B548"/>
-    <mergeCell ref="C546:C548"/>
-    <mergeCell ref="B477:B480"/>
-    <mergeCell ref="C477:C480"/>
-    <mergeCell ref="B481:B483"/>
-    <mergeCell ref="C481:C483"/>
-    <mergeCell ref="B486:B487"/>
-    <mergeCell ref="C486:C487"/>
-    <mergeCell ref="B499:B501"/>
-    <mergeCell ref="C499:C501"/>
-    <mergeCell ref="A504:A511"/>
-    <mergeCell ref="B504:B505"/>
-    <mergeCell ref="C504:C505"/>
-    <mergeCell ref="B506:B509"/>
-    <mergeCell ref="C506:C509"/>
-    <mergeCell ref="B510:B511"/>
-    <mergeCell ref="C510:C511"/>
-    <mergeCell ref="C465:C467"/>
-    <mergeCell ref="B469:B470"/>
-    <mergeCell ref="C469:C470"/>
-    <mergeCell ref="B471:B472"/>
-    <mergeCell ref="C471:C472"/>
-    <mergeCell ref="B473:B476"/>
-    <mergeCell ref="C473:C476"/>
-    <mergeCell ref="A442:A468"/>
-    <mergeCell ref="B443:B444"/>
-    <mergeCell ref="C443:C444"/>
-    <mergeCell ref="B446:B447"/>
-    <mergeCell ref="C446:C447"/>
-    <mergeCell ref="B450:B451"/>
-    <mergeCell ref="C450:C451"/>
-    <mergeCell ref="B454:B458"/>
-    <mergeCell ref="C454:C458"/>
-    <mergeCell ref="B465:B467"/>
-    <mergeCell ref="A469:A503"/>
-    <mergeCell ref="B488:B489"/>
-    <mergeCell ref="C488:C489"/>
-    <mergeCell ref="B490:B492"/>
-    <mergeCell ref="C490:C492"/>
-    <mergeCell ref="B493:B498"/>
-    <mergeCell ref="C493:C498"/>
-    <mergeCell ref="B431:B433"/>
-    <mergeCell ref="C431:C433"/>
-    <mergeCell ref="A434:A441"/>
-    <mergeCell ref="B434:B436"/>
-    <mergeCell ref="C434:C436"/>
-    <mergeCell ref="B440:B441"/>
-    <mergeCell ref="C440:C441"/>
-    <mergeCell ref="B420:B425"/>
-    <mergeCell ref="C420:C425"/>
-    <mergeCell ref="B426:B427"/>
-    <mergeCell ref="C426:C427"/>
-    <mergeCell ref="B428:B430"/>
-    <mergeCell ref="C428:C430"/>
-    <mergeCell ref="A332:A433"/>
-    <mergeCell ref="B403:B412"/>
-    <mergeCell ref="C403:C412"/>
-    <mergeCell ref="B413:B417"/>
-    <mergeCell ref="C413:C417"/>
-    <mergeCell ref="B418:B419"/>
-    <mergeCell ref="C418:C419"/>
-    <mergeCell ref="B387:B388"/>
-    <mergeCell ref="C387:C388"/>
-    <mergeCell ref="B389:B396"/>
-    <mergeCell ref="C389:C396"/>
-    <mergeCell ref="B397:B402"/>
-    <mergeCell ref="C397:C402"/>
-    <mergeCell ref="B362:B370"/>
-    <mergeCell ref="C362:C370"/>
-    <mergeCell ref="B372:B379"/>
-    <mergeCell ref="C372:C379"/>
-    <mergeCell ref="B380:B386"/>
-    <mergeCell ref="C380:C386"/>
-    <mergeCell ref="B339:B348"/>
-    <mergeCell ref="C339:C348"/>
-    <mergeCell ref="B349:B352"/>
-    <mergeCell ref="C349:C352"/>
-    <mergeCell ref="B353:B361"/>
-    <mergeCell ref="C353:C361"/>
-    <mergeCell ref="B332:B333"/>
-    <mergeCell ref="C332:C333"/>
-    <mergeCell ref="B335:B336"/>
-    <mergeCell ref="C335:C336"/>
-    <mergeCell ref="C317:C321"/>
-    <mergeCell ref="B323:B325"/>
-    <mergeCell ref="C323:C325"/>
-    <mergeCell ref="B326:B327"/>
-    <mergeCell ref="C326:C327"/>
-    <mergeCell ref="B328:B329"/>
-    <mergeCell ref="C328:C329"/>
-    <mergeCell ref="A305:A307"/>
-    <mergeCell ref="B305:B307"/>
-    <mergeCell ref="C305:C307"/>
-    <mergeCell ref="A308:A309"/>
-    <mergeCell ref="A310:A331"/>
-    <mergeCell ref="B310:B312"/>
-    <mergeCell ref="C310:C312"/>
-    <mergeCell ref="B314:B316"/>
-    <mergeCell ref="C314:C316"/>
-    <mergeCell ref="B317:B321"/>
-    <mergeCell ref="B330:B331"/>
-    <mergeCell ref="C330:C331"/>
-    <mergeCell ref="A299:A300"/>
-    <mergeCell ref="B299:B300"/>
-    <mergeCell ref="C299:C300"/>
-    <mergeCell ref="A301:A304"/>
-    <mergeCell ref="B301:B304"/>
-    <mergeCell ref="C301:C304"/>
-    <mergeCell ref="C281:C283"/>
-    <mergeCell ref="A285:A298"/>
-    <mergeCell ref="B285:B288"/>
-    <mergeCell ref="C285:C288"/>
-    <mergeCell ref="B289:B291"/>
-    <mergeCell ref="C289:C291"/>
-    <mergeCell ref="B295:B296"/>
-    <mergeCell ref="C295:C296"/>
-    <mergeCell ref="C268:C269"/>
-    <mergeCell ref="A270:A272"/>
-    <mergeCell ref="B270:B271"/>
-    <mergeCell ref="C270:C271"/>
-    <mergeCell ref="A273:A274"/>
-    <mergeCell ref="A275:A284"/>
-    <mergeCell ref="B276:B277"/>
-    <mergeCell ref="B278:B279"/>
-    <mergeCell ref="C278:C279"/>
-    <mergeCell ref="B281:B283"/>
-    <mergeCell ref="A246:A269"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="B249:B250"/>
-    <mergeCell ref="C249:C250"/>
-    <mergeCell ref="B251:B253"/>
-    <mergeCell ref="C251:C253"/>
-    <mergeCell ref="B260:B261"/>
-    <mergeCell ref="B262:B263"/>
-    <mergeCell ref="C262:C263"/>
-    <mergeCell ref="B268:B269"/>
-    <mergeCell ref="A221:A245"/>
-    <mergeCell ref="B221:B225"/>
-    <mergeCell ref="C221:C225"/>
-    <mergeCell ref="B226:B232"/>
-    <mergeCell ref="C226:C232"/>
-    <mergeCell ref="B235:B241"/>
-    <mergeCell ref="C235:C241"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:C211"/>
-    <mergeCell ref="B212:B214"/>
-    <mergeCell ref="C212:C214"/>
-    <mergeCell ref="B215:B219"/>
-    <mergeCell ref="C215:C219"/>
-    <mergeCell ref="B200:B203"/>
-    <mergeCell ref="C200:C203"/>
-    <mergeCell ref="B204:B205"/>
-    <mergeCell ref="C204:C205"/>
-    <mergeCell ref="B206:B207"/>
-    <mergeCell ref="C206:C207"/>
-    <mergeCell ref="A181:A187"/>
-    <mergeCell ref="B182:B187"/>
-    <mergeCell ref="C182:C187"/>
-    <mergeCell ref="B190:B194"/>
-    <mergeCell ref="C190:C194"/>
-    <mergeCell ref="B195:B199"/>
-    <mergeCell ref="C195:C199"/>
-    <mergeCell ref="A188:A220"/>
-    <mergeCell ref="A166:A180"/>
-    <mergeCell ref="B166:B170"/>
-    <mergeCell ref="C166:C170"/>
-    <mergeCell ref="B172:B173"/>
-    <mergeCell ref="C172:C173"/>
-    <mergeCell ref="B174:B178"/>
-    <mergeCell ref="C174:C178"/>
-    <mergeCell ref="A158:A159"/>
-    <mergeCell ref="A160:A165"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="B162:B165"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="A134:A138"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="C134:C137"/>
-    <mergeCell ref="A142:A157"/>
-    <mergeCell ref="B142:B148"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="C153:C156"/>
-    <mergeCell ref="A120:A127"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="B122:B127"/>
-    <mergeCell ref="C122:C127"/>
-    <mergeCell ref="A128:A133"/>
-    <mergeCell ref="B128:B132"/>
-    <mergeCell ref="C128:C132"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A113:A119"/>
-    <mergeCell ref="B114:B119"/>
-    <mergeCell ref="C114:C119"/>
-    <mergeCell ref="B80:B86"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="A92:A109"/>
-    <mergeCell ref="B95:B99"/>
-    <mergeCell ref="C95:C99"/>
-    <mergeCell ref="B100:B106"/>
-    <mergeCell ref="C100:C106"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="A58:A91"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="B73:B79"/>
-    <mergeCell ref="C73:C79"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="A41:A57"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="B49:B55"/>
-    <mergeCell ref="C49:C55"/>
-    <mergeCell ref="A2:A40"/>
-    <mergeCell ref="B2:B19"/>
-    <mergeCell ref="C2:C19"/>
-    <mergeCell ref="B20:B28"/>
-    <mergeCell ref="C20:C28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FDCEF4-CB77-430E-AF22-AE66FD1242FD}">
+  <dimension ref="A1:C90"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.90625" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="B2" s="4">
+        <v>97.01</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9"/>
+      <c r="B3" s="4">
+        <v>97.02</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9"/>
+      <c r="B4" s="4">
+        <v>97.03</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9"/>
+      <c r="B5" s="4">
+        <v>97.04</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9"/>
+      <c r="B6" s="4">
+        <v>97.05</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="9"/>
+      <c r="B7" s="4">
+        <v>97.06</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4">
+        <v>97.07</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9"/>
+      <c r="B9" s="4">
+        <v>97.08</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9"/>
+      <c r="B10" s="4">
+        <v>97.09</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4">
+        <v>97.1</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9"/>
+      <c r="B12" s="4">
+        <v>97.11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="9"/>
+      <c r="B13" s="4">
+        <v>97.12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4">
+        <v>97.13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9"/>
+      <c r="B15" s="4">
+        <v>97.14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4">
+        <v>97.15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9"/>
+      <c r="B17" s="4">
+        <v>97.16</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="9"/>
+      <c r="B18" s="4">
+        <v>97.17</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4">
+        <v>97.18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="9"/>
+      <c r="B20" s="4">
+        <v>97.19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="9"/>
+      <c r="B21" s="4">
+        <v>97.2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="9"/>
+      <c r="B22" s="4">
+        <v>97.21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="9"/>
+      <c r="B23" s="4">
+        <v>97.22</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="9"/>
+      <c r="B24" s="4">
+        <v>97.23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="9"/>
+      <c r="B25" s="4">
+        <v>97.24</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="9"/>
+      <c r="B26" s="4">
+        <v>97.39</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="9"/>
+      <c r="B27" s="4">
+        <v>97.4</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="4">
+        <v>97.41</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="9"/>
+      <c r="B29" s="4">
+        <v>97.42</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="9"/>
+      <c r="B30" s="4">
+        <v>97.43</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="9"/>
+      <c r="B31" s="4">
+        <v>97.44</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="9"/>
+      <c r="B32" s="4">
+        <v>97.45</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="9"/>
+      <c r="B33" s="4">
+        <v>97.46</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="9"/>
+      <c r="B34" s="4">
+        <v>97.47</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="9"/>
+      <c r="B35" s="4">
+        <v>97.48</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="9"/>
+      <c r="B36" s="4">
+        <v>97.49</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="9"/>
+      <c r="B37" s="4">
+        <v>97.5</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="9"/>
+      <c r="B38" s="4">
+        <v>97.51</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="9"/>
+      <c r="B39" s="4">
+        <v>97.52</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="9"/>
+      <c r="B40" s="4">
+        <v>97.53</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="9"/>
+      <c r="B41" s="4">
+        <v>97.54</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="9"/>
+      <c r="B42" s="4">
+        <v>97.55</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="9"/>
+      <c r="B43" s="4">
+        <v>97.56</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="9"/>
+      <c r="B44" s="4">
+        <v>97.57</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="9"/>
+      <c r="B45" s="4">
+        <v>97.58</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="9"/>
+      <c r="B46" s="4">
+        <v>97.59</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="9"/>
+      <c r="B47" s="4">
+        <v>97.6</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="9"/>
+      <c r="B48" s="4">
+        <v>97.61</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="9"/>
+      <c r="B49" s="4">
+        <v>97.62</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="9"/>
+      <c r="B50" s="4">
+        <v>97.63</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="9"/>
+      <c r="B51" s="4">
+        <v>97.64</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="9"/>
+      <c r="B52" s="4">
+        <v>97.65</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="9"/>
+      <c r="B53" s="4">
+        <v>97.66</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="9"/>
+      <c r="B54" s="4">
+        <v>97.67</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="9"/>
+      <c r="B55" s="4">
+        <v>97.68</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="9"/>
+      <c r="B56" s="4">
+        <v>97.69</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="9"/>
+      <c r="B57" s="4">
+        <v>97.7</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="9"/>
+      <c r="B58" s="4">
+        <v>97.71</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="9"/>
+      <c r="B59" s="4">
+        <v>97.72</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="9"/>
+      <c r="B60" s="4">
+        <v>97.73</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="9"/>
+      <c r="B61" s="4">
+        <v>97.74</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="9"/>
+      <c r="B62" s="4">
+        <v>97.75</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="9"/>
+      <c r="B63" s="4">
+        <v>97.76</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="9"/>
+      <c r="B64" s="4">
+        <v>97.77</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="9"/>
+      <c r="B65" s="4">
+        <v>97.78</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="9"/>
+      <c r="B66" s="4">
+        <v>97.79</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="9"/>
+      <c r="B67" s="8">
+        <v>97.8</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+    </row>
+    <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="B69" s="4">
+        <v>99.14</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="9"/>
+      <c r="B70" s="4">
+        <v>99.15</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="9"/>
+      <c r="B71" s="4">
+        <v>99.16</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="9"/>
+      <c r="B72" s="4">
+        <v>99.17</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="9"/>
+      <c r="B73" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="9"/>
+      <c r="B74" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="9"/>
+      <c r="B75" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="9"/>
+      <c r="B76" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="9"/>
+      <c r="B77" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="9"/>
+      <c r="B78" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="9"/>
+      <c r="B79" s="4">
+        <v>99.18</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="9"/>
+      <c r="B80" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="9"/>
+      <c r="B81" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="9"/>
+      <c r="B82" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="9"/>
+      <c r="B83" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="9"/>
+      <c r="B84" s="4">
+        <v>99.19</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="9"/>
+      <c r="B85" s="4">
+        <v>99.8</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="9"/>
+      <c r="B86" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="9"/>
+      <c r="B87" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="9"/>
+      <c r="B88" s="4">
+        <v>99.81</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="9"/>
+      <c r="B89" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="10"/>
+      <c r="B90" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>709</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A69:A90"/>
+    <mergeCell ref="A2:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>